<commit_message>
AutoCommit_16 октября 2023 г. 12:15:17_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
   <si>
-    <t>11сен</t>
-  </si>
-  <si>
     <t>Басманов Кирилл</t>
   </si>
   <si>
@@ -123,10 +120,19 @@
     <t>ОК</t>
   </si>
   <si>
-    <t>ДЗ2</t>
-  </si>
-  <si>
     <t>ДЗ</t>
+  </si>
+  <si>
+    <t>дз2</t>
+  </si>
+  <si>
+    <t>дз4</t>
+  </si>
+  <si>
+    <t>дз5</t>
+  </si>
+  <si>
+    <t>дз6</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -188,11 +194,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -205,6 +220,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -512,10 +530,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -552,16 +570,22 @@
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
+      <c r="G3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
@@ -570,43 +594,53 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -617,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -631,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -643,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -655,11 +689,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -669,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -681,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -695,11 +729,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -709,7 +743,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -721,73 +755,73 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -796,64 +830,72 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -862,15 +904,15 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
@@ -878,62 +920,71 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -947,7 +998,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_16 октября 2023 г. 13:51:33_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -218,11 +218,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -530,10 +530,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -544,29 +544,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -581,10 +581,10 @@
       <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -642,11 +642,23 @@
       <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -660,7 +672,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -672,19 +684,28 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -860,11 +881,13 @@
       <c r="C23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -876,7 +899,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -887,10 +910,17 @@
         <v>32</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -953,7 +983,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -965,7 +995,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -976,10 +1006,20 @@
         <v>32</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_27 октября 2023 г. 8:28:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -550,7 +550,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -902,6 +902,12 @@
         <v>32</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_27 октября 2023 г. 8:29:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -819,7 +819,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -831,7 +831,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -871,7 +871,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -911,7 +911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -930,7 +930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -963,7 +963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1061,8 +1061,11 @@
       <c r="H31" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_27 октября 2023 г. 10:40:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -686,8 +686,16 @@
         <v>32</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -696,10 +704,15 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -763,7 +776,9 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -819,7 +834,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -831,19 +846,24 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -857,7 +877,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -867,9 +887,14 @@
       <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -924,7 +949,9 @@
       <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
         <v>32</v>
@@ -937,7 +964,9 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -959,7 +988,13 @@
       <c r="F25" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -970,7 +1005,9 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2">
         <v>5</v>
@@ -987,11 +1024,21 @@
       <c r="C27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
AutoCommit_30 октября 2023 г. 12:13:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -550,7 +550,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -619,9 +619,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -890,7 +903,9 @@
       <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="H20" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
AutoCommit_30 октября 2023 г. 12:18:02_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -996,7 +996,9 @@
       <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_30 октября 2023 г. 14:02:50_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -698,15 +698,22 @@
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -721,8 +728,15 @@
         <v>32</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>32</v>
       </c>
@@ -750,6 +764,9 @@
       <c r="H10" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -765,7 +782,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -777,7 +794,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -787,13 +804,21 @@
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -807,7 +832,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -833,7 +858,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -843,9 +868,16 @@
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -869,10 +901,22 @@
       <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1097,7 +1141,9 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_31 октября 2023 г. 17:28:10_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1145,8 +1145,18 @@
         <v>32</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">

</xml_diff>

<commit_message>
AutoCommit_1 ноября 2023 г. 14:11:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>ок</t>
+  </si>
+  <si>
+    <t>оок</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1192,8 +1195,12 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E32" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_2 ноября 2023 г. 12:27:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1072,11 +1072,24 @@
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">

</xml_diff>

<commit_message>
AutoCommit_3 ноября 2023 г. 8:42:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -550,10 +550,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -621,14 +621,18 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 ноября 2023 г. 9:34:48_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -550,10 +550,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,9 @@
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
@@ -745,6 +747,9 @@
         <v>32</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -758,7 +763,9 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
@@ -937,9 +944,24 @@
       <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -957,7 +979,12 @@
       <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>32</v>
       </c>
@@ -969,12 +996,18 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1131,11 +1164,16 @@
       <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -1149,10 +1187,27 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 10:06:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1008,6 +1008,12 @@
       <c r="F21" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1066,9 +1072,21 @@
       <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 10:07:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1113,9 +1113,7 @@
       <c r="H25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 11:46:23_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -803,10 +803,19 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 12:16:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="42">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -559,7 +559,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,9 @@
       <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 13:50:59_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="42">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -556,10 +556,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1083,13 @@
       <c r="E23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G23" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1321,9 +1324,15 @@
       <c r="E32" s="2">
         <v>5</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 ноября 2023 г. 10:02:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -548,7 +548,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1234,6 +1234,9 @@
       <c r="F24" s="2">
         <v>5</v>
       </c>
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
       <c r="H24" s="2">
         <v>5</v>
       </c>
@@ -1242,7 +1245,7 @@
       </c>
       <c r="L24" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N24">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_22 ноября 2023 г. 8:58:11_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -163,12 +163,24 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -218,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -232,12 +244,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -545,10 +567,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="I31" activeCellId="2" sqref="I28 I29 I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -559,29 +581,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -622,25 +644,25 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="C5" s="6">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6">
         <v>5</v>
       </c>
       <c r="L5">
@@ -658,28 +680,28 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6">
         <v>5</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <f t="shared" ref="L6:L33" si="0">SUM(C6:I6)</f>
         <v>30</v>
       </c>
@@ -694,25 +716,25 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5</v>
+      </c>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -727,28 +749,28 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="L8" s="6">
+      <c r="C8" s="6">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>5</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -763,28 +785,28 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2">
-        <v>5</v>
-      </c>
-      <c r="L9" s="6">
+      <c r="C9" s="6">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+      <c r="F9" s="6">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -799,28 +821,28 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2">
-        <v>5</v>
-      </c>
-      <c r="I10" s="2">
-        <v>5</v>
-      </c>
-      <c r="L10" s="6">
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>5</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -828,24 +850,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="L11" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N11">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="L11" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N11" s="12">
         <v>3</v>
       </c>
     </row>
@@ -856,20 +878,20 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
         <v>5</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="F12" s="6">
+        <v>5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>5</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -884,25 +906,25 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="C13" s="6">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>5</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -910,24 +932,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="L14" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N14">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11">
+        <v>5</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="L14" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N14" s="12">
         <v>3</v>
       </c>
     </row>
@@ -938,25 +960,25 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
-        <v>5</v>
-      </c>
-      <c r="G15" s="5">
-        <v>5</v>
-      </c>
-      <c r="H15" s="5">
-        <v>5</v>
-      </c>
-      <c r="L15" s="6">
+      <c r="C15" s="6">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5</v>
+      </c>
+      <c r="E15" s="6">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7">
+        <v>5</v>
+      </c>
+      <c r="H15" s="7">
+        <v>5</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -971,20 +993,20 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="C16" s="6">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6">
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="H16" s="2">
-        <v>5</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="H16" s="6">
+        <v>5</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1003,7 +1025,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1018,28 +1040,28 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2">
-        <v>5</v>
-      </c>
-      <c r="L18" s="6">
+      <c r="C18" s="6">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6">
+        <v>5</v>
+      </c>
+      <c r="G18" s="6">
+        <v>5</v>
+      </c>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>5</v>
+      </c>
+      <c r="L18" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1054,28 +1076,28 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2">
-        <v>5</v>
-      </c>
-      <c r="I19" s="2">
-        <v>5</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="C19" s="6">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6">
+        <v>5</v>
+      </c>
+      <c r="H19" s="6">
+        <v>5</v>
+      </c>
+      <c r="I19" s="6">
+        <v>5</v>
+      </c>
+      <c r="L19" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1090,25 +1112,25 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2">
-        <v>5</v>
-      </c>
-      <c r="L20" s="6">
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6">
+        <v>5</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6">
+        <v>5</v>
+      </c>
+      <c r="H20" s="6">
+        <v>5</v>
+      </c>
+      <c r="L20" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1123,25 +1145,25 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2">
-        <v>5</v>
-      </c>
-      <c r="L21" s="6">
+      <c r="C21" s="6">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6">
+        <v>5</v>
+      </c>
+      <c r="F21" s="6">
+        <v>5</v>
+      </c>
+      <c r="G21" s="6">
+        <v>5</v>
+      </c>
+      <c r="H21" s="6">
+        <v>5</v>
+      </c>
+      <c r="L21" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1156,25 +1178,25 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>5</v>
-      </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2">
-        <v>5</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="C22" s="6">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+      <c r="E22" s="6">
+        <v>5</v>
+      </c>
+      <c r="F22" s="6">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6">
+        <v>5</v>
+      </c>
+      <c r="L22" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1189,25 +1211,25 @@
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="C23" s="6">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6">
+        <v>5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="6">
+        <v>5</v>
+      </c>
+      <c r="H23" s="6">
+        <v>5</v>
+      </c>
+      <c r="L23" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1222,28 +1244,28 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2">
-        <v>5</v>
-      </c>
-      <c r="G24" s="5">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="2">
-        <v>5</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="C24" s="6">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>5</v>
+      </c>
+      <c r="F24" s="6">
+        <v>5</v>
+      </c>
+      <c r="G24" s="7">
+        <v>5</v>
+      </c>
+      <c r="H24" s="6">
+        <v>5</v>
+      </c>
+      <c r="I24" s="6">
+        <v>5</v>
+      </c>
+      <c r="L24" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1258,26 +1280,26 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
-        <v>5</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="C25" s="6">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6">
+        <v>5</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5</v>
+      </c>
+      <c r="H25" s="6">
         <v>5</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="L25" s="6">
+      <c r="L25" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1292,28 +1314,28 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
-        <v>5</v>
-      </c>
-      <c r="G26" s="2">
-        <v>5</v>
-      </c>
-      <c r="H26" s="2">
-        <v>5</v>
-      </c>
-      <c r="I26" s="2">
-        <v>5</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6">
+        <v>5</v>
+      </c>
+      <c r="G26" s="6">
+        <v>5</v>
+      </c>
+      <c r="H26" s="6">
+        <v>5</v>
+      </c>
+      <c r="I26" s="6">
+        <v>5</v>
+      </c>
+      <c r="L26" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1328,25 +1350,25 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2">
-        <v>5</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="C27" s="6">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5</v>
+      </c>
+      <c r="F27" s="6">
+        <v>5</v>
+      </c>
+      <c r="G27" s="6">
+        <v>5</v>
+      </c>
+      <c r="H27" s="6">
+        <v>5</v>
+      </c>
+      <c r="L27" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1361,28 +1383,28 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
-        <v>5</v>
-      </c>
-      <c r="G28" s="2">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2">
-        <v>5</v>
-      </c>
-      <c r="I28" s="2">
-        <v>5</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="C28" s="6">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6">
+        <v>5</v>
+      </c>
+      <c r="F28" s="6">
+        <v>5</v>
+      </c>
+      <c r="G28" s="6">
+        <v>5</v>
+      </c>
+      <c r="H28" s="6">
+        <v>5</v>
+      </c>
+      <c r="I28" s="6">
+        <v>5</v>
+      </c>
+      <c r="L28" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1397,28 +1419,28 @@
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2">
-        <v>5</v>
-      </c>
-      <c r="G29" s="2">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <v>5</v>
-      </c>
-      <c r="I29" s="2">
-        <v>5</v>
-      </c>
-      <c r="L29" s="6">
+      <c r="C29" s="6">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6">
+        <v>5</v>
+      </c>
+      <c r="F29" s="6">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6">
+        <v>5</v>
+      </c>
+      <c r="H29" s="6">
+        <v>5</v>
+      </c>
+      <c r="I29" s="6">
+        <v>5</v>
+      </c>
+      <c r="L29" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1433,23 +1455,23 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="6">
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2">
-        <v>5</v>
-      </c>
-      <c r="G30" s="2">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2">
-        <v>5</v>
-      </c>
-      <c r="L30" s="6">
+      <c r="E30" s="6">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6">
+        <v>5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>5</v>
+      </c>
+      <c r="H30" s="6">
+        <v>5</v>
+      </c>
+      <c r="L30" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1464,26 +1486,26 @@
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="6">
         <v>5</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2">
-        <v>5</v>
-      </c>
-      <c r="G31" s="2">
-        <v>5</v>
-      </c>
-      <c r="H31" s="2">
-        <v>5</v>
-      </c>
-      <c r="I31" s="2">
-        <v>5</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="E31" s="6">
+        <v>5</v>
+      </c>
+      <c r="F31" s="6">
+        <v>5</v>
+      </c>
+      <c r="G31" s="6">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6">
+        <v>5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>5</v>
+      </c>
+      <c r="L31" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1498,23 +1520,23 @@
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2">
-        <v>5</v>
-      </c>
-      <c r="F32" s="2">
-        <v>5</v>
-      </c>
-      <c r="G32" s="2">
+      <c r="C32" s="6">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6">
+        <v>5</v>
+      </c>
+      <c r="F32" s="6">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6">
         <v>5</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="L32" s="6">
+      <c r="L32" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1533,7 +1555,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="L33" s="6">
+      <c r="L33" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 20:49:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -163,7 +163,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -251,8 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -260,6 +264,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -567,10 +576,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I31" activeCellId="2" sqref="I28 I29 I31"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -581,29 +590,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -701,6 +710,9 @@
       <c r="J6" s="2">
         <v>5</v>
       </c>
+      <c r="K6" s="11">
+        <v>5</v>
+      </c>
       <c r="L6" s="5">
         <f t="shared" ref="L6:L33" si="0">SUM(C6:I6)</f>
         <v>30</v>
@@ -850,24 +862,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+    <row r="11" spans="1:23" s="10" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>7</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11">
-        <v>5</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="L11" s="12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N11" s="12">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="L11" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N11" s="10">
         <v>3</v>
       </c>
     </row>
@@ -932,24 +944,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+    <row r="14" spans="1:23" s="10" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11">
-        <v>5</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="L14" s="12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N14" s="12">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="L14" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N14" s="10">
         <v>3</v>
       </c>
     </row>
@@ -1551,13 +1563,19 @@
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="C33" s="2">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2">
+        <v>5</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="L33" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N33">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 12:37:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
+    <sheet name="Диаграмма1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sibirev I. V." sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -133,6 +134,9 @@
   </si>
   <si>
     <t>дз8</t>
+  </si>
+  <si>
+    <t>вариант</t>
   </si>
 </sst>
 </file>
@@ -236,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -269,6 +273,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -284,6 +291,830 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sibirev I. V.'!$M$8:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="147681608"/>
+        <c:axId val="147680432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="147681608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="147680432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="147680432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="147681608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9295694" cy="6041319"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,10 +1407,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -639,6 +1470,9 @@
       <c r="J3" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="M3" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
@@ -674,12 +1508,8 @@
       <c r="I5" s="6">
         <v>5</v>
       </c>
-      <c r="L5">
-        <f>SUM(C5:I5)</f>
-        <v>35</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
+      <c r="M5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -713,13 +1543,7 @@
       <c r="K6" s="11">
         <v>5</v>
       </c>
-      <c r="L6" s="5">
-        <f t="shared" ref="L6:L33" si="0">SUM(C6:I6)</f>
-        <v>30</v>
-      </c>
-      <c r="N6">
-        <v>5</v>
-      </c>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -746,13 +1570,7 @@
       <c r="H7" s="6">
         <v>5</v>
       </c>
-      <c r="L7" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N7">
-        <v>5</v>
-      </c>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -782,12 +1600,9 @@
       <c r="I8" s="6">
         <v>5</v>
       </c>
-      <c r="L8" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N8">
-        <v>5</v>
+      <c r="L8" s="5"/>
+      <c r="M8">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -818,12 +1633,9 @@
       <c r="I9" s="6">
         <v>5</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N9">
-        <v>5</v>
+      <c r="L9" s="5"/>
+      <c r="M9">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -854,12 +1666,9 @@
       <c r="I10" s="6">
         <v>5</v>
       </c>
-      <c r="L10" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N10">
-        <v>5</v>
+      <c r="L10" s="5"/>
+      <c r="M10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="10" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -875,13 +1684,6 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="L11" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N11" s="10">
-        <v>3</v>
-      </c>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -903,13 +1705,7 @@
       <c r="G12" s="6">
         <v>5</v>
       </c>
-      <c r="L12" s="5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -936,12 +1732,9 @@
       <c r="H13" s="6">
         <v>5</v>
       </c>
-      <c r="L13" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N13">
-        <v>5</v>
+      <c r="L13" s="5"/>
+      <c r="M13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="10" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,13 +1750,6 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="L14" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N14" s="10">
-        <v>3</v>
-      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -990,12 +1776,9 @@
       <c r="H15" s="7">
         <v>5</v>
       </c>
-      <c r="L15" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N15">
-        <v>5</v>
+      <c r="L15" s="5"/>
+      <c r="M15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1018,15 +1801,9 @@
       <c r="H16" s="6">
         <v>5</v>
       </c>
-      <c r="L16" s="5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1037,15 +1814,12 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="L17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="5"/>
+      <c r="M17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1073,15 +1847,12 @@
       <c r="I18" s="6">
         <v>5</v>
       </c>
-      <c r="L18" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="5"/>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1109,15 +1880,9 @@
       <c r="I19" s="6">
         <v>5</v>
       </c>
-      <c r="L19" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1142,15 +1907,12 @@
       <c r="H20" s="6">
         <v>5</v>
       </c>
-      <c r="L20" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="5"/>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1175,15 +1937,9 @@
       <c r="H21" s="6">
         <v>5</v>
       </c>
-      <c r="L21" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1208,15 +1964,12 @@
       <c r="H22" s="6">
         <v>5</v>
       </c>
-      <c r="L22" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="5"/>
+      <c r="M22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1241,15 +1994,9 @@
       <c r="H23" s="6">
         <v>5</v>
       </c>
-      <c r="L23" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1277,15 +2024,12 @@
       <c r="I24" s="6">
         <v>5</v>
       </c>
-      <c r="L24" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="5"/>
+      <c r="M24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1311,15 +2055,12 @@
         <v>5</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="L25" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="5"/>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1347,15 +2088,9 @@
       <c r="I26" s="6">
         <v>5</v>
       </c>
-      <c r="L26" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1380,15 +2115,9 @@
       <c r="H27" s="6">
         <v>5</v>
       </c>
-      <c r="L27" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1416,15 +2145,9 @@
       <c r="I28" s="6">
         <v>5</v>
       </c>
-      <c r="L28" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1452,15 +2175,9 @@
       <c r="I29" s="6">
         <v>5</v>
       </c>
-      <c r="L29" s="5">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1483,15 +2200,9 @@
       <c r="H30" s="6">
         <v>5</v>
       </c>
-      <c r="L30" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="N30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1517,15 +2228,12 @@
       <c r="I31" s="6">
         <v>5</v>
       </c>
-      <c r="L31" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L31" s="5"/>
+      <c r="M31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1548,15 +2256,9 @@
         <v>5</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="L32" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="N32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -1573,15 +2275,9 @@
         <v>5</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="L33" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="N33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C34" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 12:55:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -271,11 +271,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -308,7 +308,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -387,11 +386,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="147681608"/>
-        <c:axId val="147680432"/>
+        <c:axId val="161816120"/>
+        <c:axId val="117483944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147681608"/>
+        <c:axId val="161816120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +432,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147680432"/>
+        <c:crossAx val="117483944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147680432"/>
+        <c:axId val="117483944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +491,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147681608"/>
+        <c:crossAx val="161816120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1407,10 +1406,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1421,29 +1420,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -1470,7 +1469,7 @@
       <c r="J3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="12" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2116,6 +2115,9 @@
         <v>5</v>
       </c>
       <c r="L27" s="5"/>
+      <c r="M27">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -2257,6 +2259,9 @@
       </c>
       <c r="H32" s="2"/>
       <c r="L32" s="5"/>
+      <c r="M32">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 8:40:38_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -387,11 +387,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="162009752"/>
-        <c:axId val="161910352"/>
+        <c:axId val="152822232"/>
+        <c:axId val="152823408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162009752"/>
+        <c:axId val="152822232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +433,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161910352"/>
+        <c:crossAx val="152823408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161910352"/>
+        <c:axId val="152823408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +492,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162009752"/>
+        <c:crossAx val="152822232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,7 +1410,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="Q4" s="13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1634,6 +1634,9 @@
         <v>5</v>
       </c>
       <c r="L7" s="5"/>
+      <c r="M7">
+        <v>4</v>
+      </c>
       <c r="N7" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1648,7 +1651,7 @@
       </c>
       <c r="Q7" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2136,6 +2139,9 @@
         <v>5</v>
       </c>
       <c r="L19" s="5"/>
+      <c r="M19">
+        <v>4</v>
+      </c>
       <c r="N19" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2150,7 +2156,7 @@
       </c>
       <c r="Q19" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 10:16:15_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -387,11 +387,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="152822232"/>
-        <c:axId val="152823408"/>
+        <c:axId val="114347824"/>
+        <c:axId val="154170584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152822232"/>
+        <c:axId val="114347824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +433,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152823408"/>
+        <c:crossAx val="154170584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152823408"/>
+        <c:axId val="154170584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +492,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152822232"/>
+        <c:crossAx val="114347824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,7 +1410,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="P4" s="13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q4" s="13">
         <f t="shared" si="0"/>
@@ -1581,6 +1581,9 @@
       <c r="H6" s="6">
         <v>5</v>
       </c>
+      <c r="I6" s="7">
+        <v>5</v>
+      </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
@@ -2036,9 +2039,15 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="L17" s="5"/>
       <c r="M17">
@@ -2765,8 +2774,16 @@
       <c r="E33" s="2">
         <v>5</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2">
+        <v>5</v>
+      </c>
+      <c r="H33" s="11">
+        <v>5</v>
+      </c>
       <c r="L33" s="5"/>
+      <c r="M33">
+        <v>3</v>
+      </c>
       <c r="N33" s="13">
         <f t="shared" ref="N33:Q33" si="3">IF($M33=N$3,1,0)</f>
         <v>0</v>
@@ -2777,7 +2794,7 @@
       </c>
       <c r="P33" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="13">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
AutoCommit_9 декабря 2023 г. 15:27:44_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -387,11 +387,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="114347824"/>
-        <c:axId val="154170584"/>
+        <c:axId val="146807120"/>
+        <c:axId val="146807512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114347824"/>
+        <c:axId val="146807120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +433,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154170584"/>
+        <c:crossAx val="146807512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154170584"/>
+        <c:axId val="146807512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +492,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114347824"/>
+        <c:crossAx val="146807120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,7 +1410,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
       <c r="F4" s="1"/>
       <c r="N4">
         <f>SUM(N5:N34)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" ref="O4:Q4" si="0">SUM(O5:O34)</f>
@@ -1855,9 +1855,12 @@
         <v>5</v>
       </c>
       <c r="L12" s="5"/>
+      <c r="M12">
+        <v>1</v>
+      </c>
       <c r="N12" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 12:43:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -403,11 +403,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="146518560"/>
-        <c:axId val="146521000"/>
+        <c:axId val="165297824"/>
+        <c:axId val="165302312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146518560"/>
+        <c:axId val="165297824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146521000"/>
+        <c:crossAx val="165302312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146521000"/>
+        <c:axId val="165302312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +508,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146518560"/>
+        <c:crossAx val="165297824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1423,10 +1423,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1869,7 +1869,9 @@
       <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
       <c r="F12" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 22:54:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>вариант</t>
+  </si>
+  <si>
+    <t>дз9</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,25 +280,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -406,11 +401,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="153245144"/>
-        <c:axId val="153242792"/>
+        <c:axId val="160547504"/>
+        <c:axId val="160548288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153245144"/>
+        <c:axId val="160547504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +447,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153242792"/>
+        <c:crossAx val="160548288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -460,7 +455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153242792"/>
+        <c:axId val="160548288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +506,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153245144"/>
+        <c:crossAx val="160547504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1429,7 +1424,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1440,29 +1435,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
+      <c r="C1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -1489,7 +1484,10 @@
       <c r="J3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="K3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="N3">
@@ -1514,15 +1512,15 @@
         <f>SUM(N5:N34)</f>
         <v>6</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
         <f t="shared" ref="O4:Q4" si="0">SUM(O5:O34)</f>
         <v>5</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1555,7 +1553,7 @@
       <c r="I5" s="6">
         <v>5</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="7">
         <v>5</v>
       </c>
       <c r="M5">
@@ -1565,15 +1563,15 @@
         <f>IF($M5=N$3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f t="shared" ref="O5:Q20" si="1">IF($M5=O$3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P5" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="13">
+      <c r="P5" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1606,29 +1604,29 @@
       <c r="I6" s="7">
         <v>5</v>
       </c>
-      <c r="J6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="11">
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="7">
         <v>5</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6">
         <v>4</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="12">
         <f t="shared" ref="N6:Q32" si="2">IF($M6=N$3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="13">
+      <c r="O6" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1661,29 +1659,29 @@
       <c r="H7" s="6">
         <v>5</v>
       </c>
-      <c r="I7" s="17">
-        <v>5</v>
-      </c>
-      <c r="J7" s="17">
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
         <v>5</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7">
         <v>4</v>
       </c>
-      <c r="N7" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="13">
+      <c r="N7" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1720,19 +1718,19 @@
       <c r="M8">
         <v>4</v>
       </c>
-      <c r="N8" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="13">
+      <c r="N8" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1769,19 +1767,19 @@
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q9" s="13">
+      <c r="N9" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q9" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1818,19 +1816,19 @@
       <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="13">
+      <c r="N10" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1848,19 +1846,19 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="N11" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="13">
+      <c r="N11" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1878,7 +1876,7 @@
       <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="6">
         <v>5</v>
       </c>
       <c r="F12" s="6">
@@ -1891,19 +1889,19 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="13">
+      <c r="N12" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1937,19 +1935,19 @@
       <c r="M13">
         <v>3</v>
       </c>
-      <c r="N13" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q13" s="13">
+      <c r="N13" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1967,19 +1965,19 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="N14" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="13">
+      <c r="N14" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2009,27 +2007,27 @@
       <c r="H15" s="7">
         <v>5</v>
       </c>
-      <c r="I15" s="11">
-        <v>5</v>
-      </c>
-      <c r="J15" s="16"/>
+      <c r="I15" s="7">
+        <v>5</v>
+      </c>
+      <c r="J15" s="13"/>
       <c r="L15" s="5"/>
       <c r="M15">
         <v>2</v>
       </c>
-      <c r="N15" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P15" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="13">
+      <c r="N15" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2055,19 +2053,19 @@
         <v>5</v>
       </c>
       <c r="L16" s="5"/>
-      <c r="N16" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="13">
+      <c r="N16" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2079,13 +2077,13 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="C17" s="6">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6">
         <v>5</v>
       </c>
       <c r="F17" s="2"/>
@@ -2093,19 +2091,19 @@
       <c r="M17">
         <v>3</v>
       </c>
-      <c r="N17" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q17" s="13">
+      <c r="N17" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q17" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2142,19 +2140,19 @@
       <c r="M18">
         <v>1</v>
       </c>
-      <c r="N18" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="13">
+      <c r="N18" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2191,19 +2189,19 @@
       <c r="M19">
         <v>4</v>
       </c>
-      <c r="N19" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="13">
+      <c r="N19" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2237,19 +2235,19 @@
       <c r="M20">
         <v>1</v>
       </c>
-      <c r="N20" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="13">
+      <c r="N20" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2280,19 +2278,19 @@
         <v>5</v>
       </c>
       <c r="L21" s="5"/>
-      <c r="N21" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="13">
+      <c r="N21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2326,19 +2324,19 @@
       <c r="M22">
         <v>3</v>
       </c>
-      <c r="N22" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q22" s="13">
+      <c r="N22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2372,19 +2370,19 @@
       <c r="M23">
         <v>1</v>
       </c>
-      <c r="N23" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O23" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="13">
+      <c r="N23" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2421,19 +2419,19 @@
       <c r="M24">
         <v>2</v>
       </c>
-      <c r="N24" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P24" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="13">
+      <c r="N24" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P24" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2463,29 +2461,29 @@
       <c r="H25" s="6">
         <v>5</v>
       </c>
-      <c r="I25" s="2">
-        <v>5</v>
-      </c>
-      <c r="J25" s="11">
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="7">
         <v>5</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25">
         <v>1</v>
       </c>
-      <c r="N25" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O25" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="13">
+      <c r="N25" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O25" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2525,19 +2523,19 @@
       <c r="M26">
         <v>4</v>
       </c>
-      <c r="N26" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="13">
+      <c r="N26" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2571,19 +2569,19 @@
       <c r="M27">
         <v>2</v>
       </c>
-      <c r="N27" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P27" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="13">
+      <c r="N27" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P27" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2620,19 +2618,19 @@
       <c r="M28">
         <v>2</v>
       </c>
-      <c r="N28" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P28" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="13">
+      <c r="N28" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P28" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2666,19 +2664,19 @@
         <v>5</v>
       </c>
       <c r="L29" s="5"/>
-      <c r="N29" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="13">
+      <c r="N29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2707,19 +2705,19 @@
         <v>5</v>
       </c>
       <c r="L30" s="5"/>
-      <c r="N30" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="13">
+      <c r="N30" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2754,19 +2752,19 @@
       <c r="M31">
         <v>1</v>
       </c>
-      <c r="N31" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O31" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="13">
+      <c r="N31" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O31" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2798,19 +2796,19 @@
       <c r="M32">
         <v>3</v>
       </c>
-      <c r="N32" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O32" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q32" s="13">
+      <c r="N32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q32" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2822,47 +2820,47 @@
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2">
-        <v>5</v>
-      </c>
-      <c r="D33" s="14">
-        <v>5</v>
-      </c>
-      <c r="E33" s="14">
-        <v>5</v>
-      </c>
-      <c r="F33" s="14">
-        <v>5</v>
-      </c>
-      <c r="G33" s="11">
-        <v>5</v>
-      </c>
-      <c r="H33" s="11">
-        <v>5</v>
-      </c>
-      <c r="I33" s="15">
-        <v>5</v>
-      </c>
-      <c r="J33" s="16">
+      <c r="C33" s="6">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6">
+        <v>5</v>
+      </c>
+      <c r="E33" s="6">
+        <v>5</v>
+      </c>
+      <c r="F33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="7">
+        <v>5</v>
+      </c>
+      <c r="H33" s="7">
+        <v>5</v>
+      </c>
+      <c r="I33" s="16">
+        <v>5</v>
+      </c>
+      <c r="J33" s="17">
         <v>5</v>
       </c>
       <c r="L33" s="5"/>
       <c r="M33">
         <v>3</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N33" s="12">
         <f t="shared" ref="N33:Q33" si="3">IF($M33=N$3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O33" s="13">
+      <c r="O33" s="12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P33" s="13">
+      <c r="P33" s="12">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q33" s="13">
+      <c r="Q33" s="12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 19:17:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -412,11 +412,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="154356600"/>
-        <c:axId val="154359048"/>
+        <c:axId val="153000456"/>
+        <c:axId val="152999280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154356600"/>
+        <c:axId val="153000456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +458,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154359048"/>
+        <c:crossAx val="152999280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -466,7 +466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154359048"/>
+        <c:axId val="152999280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +517,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154356600"/>
+        <c:crossAx val="153000456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1432,10 +1432,10 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1443,8 @@
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="19.90625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="6" width="5.1796875" customWidth="1"/>
+    <col min="4" max="12" width="5.453125" customWidth="1"/>
+    <col min="15" max="18" width="3.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1555,19 +1556,19 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <f>IF($N4=O$2,1,0)</f>
+        <f t="shared" ref="O4:R32" si="1">IF($N4=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P4" s="12">
-        <f>IF($N4=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q4" s="12">
-        <f>IF($N4=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R4" s="12">
-        <f>IF($N4=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1610,19 +1611,19 @@
         <v>4</v>
       </c>
       <c r="O5" s="12">
-        <f>IF($N5=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5" s="12">
-        <f>IF($N5=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q5" s="12">
-        <f>IF($N5=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R5" s="12">
-        <f>IF($N5=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T5">
@@ -1665,19 +1666,19 @@
         <v>4</v>
       </c>
       <c r="O6" s="12">
-        <f>IF($N6=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P6" s="12">
-        <f>IF($N6=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q6" s="12">
-        <f>IF($N6=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R6" s="12">
-        <f>IF($N6=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1714,19 +1715,19 @@
         <v>4</v>
       </c>
       <c r="O7" s="12">
-        <f>IF($N7=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7" s="12">
-        <f>IF($N7=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q7" s="12">
-        <f>IF($N7=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R7" s="12">
-        <f>IF($N7=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1763,19 +1764,19 @@
         <v>3</v>
       </c>
       <c r="O8" s="12">
-        <f>IF($N8=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P8" s="12">
-        <f>IF($N8=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q8" s="12">
-        <f>IF($N8=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R8" s="12">
-        <f>IF($N8=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1812,19 +1813,19 @@
         <v>3</v>
       </c>
       <c r="O9" s="12">
-        <f>IF($N9=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P9" s="12">
-        <f>IF($N9=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q9" s="12">
-        <f>IF($N9=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R9" s="12">
-        <f>IF($N9=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1842,19 +1843,19 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="O10" s="12">
-        <f>IF($N10=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P10" s="12">
-        <f>IF($N10=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q10" s="12">
-        <f>IF($N10=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R10" s="12">
-        <f>IF($N10=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1885,19 +1886,19 @@
         <v>1</v>
       </c>
       <c r="O11" s="12">
-        <f>IF($N11=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P11" s="12">
-        <f>IF($N11=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q11" s="12">
-        <f>IF($N11=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R11" s="12">
-        <f>IF($N11=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1931,19 +1932,19 @@
         <v>3</v>
       </c>
       <c r="O12" s="12">
-        <f>IF($N12=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P12" s="12">
-        <f>IF($N12=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q12" s="12">
-        <f>IF($N12=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R12" s="12">
-        <f>IF($N12=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1961,19 +1962,19 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="O13" s="12">
-        <f>IF($N13=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P13" s="12">
-        <f>IF($N13=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q13" s="12">
-        <f>IF($N13=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R13" s="12">
-        <f>IF($N13=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2011,19 +2012,19 @@
         <v>2</v>
       </c>
       <c r="O14" s="12">
-        <f>IF($N14=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14" s="12">
-        <f>IF($N14=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q14" s="12">
-        <f>IF($N14=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="12">
-        <f>IF($N14=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2049,19 +2050,19 @@
       </c>
       <c r="M15" s="5"/>
       <c r="O15" s="12">
-        <f>IF($N15=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P15" s="12">
-        <f>IF($N15=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q15" s="12">
-        <f>IF($N15=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R15" s="12">
-        <f>IF($N15=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2087,19 +2088,19 @@
         <v>3</v>
       </c>
       <c r="O16" s="12">
-        <f>IF($N16=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="12">
-        <f>IF($N16=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q16" s="12">
-        <f>IF($N16=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R16" s="12">
-        <f>IF($N16=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2136,19 +2137,19 @@
         <v>1</v>
       </c>
       <c r="O17" s="12">
-        <f>IF($N17=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P17" s="12">
-        <f>IF($N17=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q17" s="12">
-        <f>IF($N17=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R17" s="12">
-        <f>IF($N17=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2185,19 +2186,19 @@
         <v>4</v>
       </c>
       <c r="O18" s="12">
-        <f>IF($N18=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" s="12">
-        <f>IF($N18=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q18" s="12">
-        <f>IF($N18=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R18" s="12">
-        <f>IF($N18=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2231,19 +2232,19 @@
         <v>1</v>
       </c>
       <c r="O19" s="12">
-        <f>IF($N19=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P19" s="12">
-        <f>IF($N19=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q19" s="12">
-        <f>IF($N19=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R19" s="12">
-        <f>IF($N19=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2274,19 +2275,19 @@
       </c>
       <c r="M20" s="5"/>
       <c r="O20" s="12">
-        <f>IF($N20=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="12">
-        <f>IF($N20=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q20" s="12">
-        <f>IF($N20=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R20" s="12">
-        <f>IF($N20=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2320,19 +2321,19 @@
         <v>3</v>
       </c>
       <c r="O21" s="12">
-        <f>IF($N21=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="12">
-        <f>IF($N21=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q21" s="12">
-        <f>IF($N21=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R21" s="12">
-        <f>IF($N21=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2366,19 +2367,19 @@
         <v>1</v>
       </c>
       <c r="O22" s="12">
-        <f>IF($N22=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P22" s="12">
-        <f>IF($N22=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q22" s="12">
-        <f>IF($N22=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R22" s="12">
-        <f>IF($N22=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2415,19 +2416,19 @@
         <v>2</v>
       </c>
       <c r="O23" s="12">
-        <f>IF($N23=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="12">
-        <f>IF($N23=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q23" s="12">
-        <f>IF($N23=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R23" s="12">
-        <f>IF($N23=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2467,19 +2468,19 @@
         <v>1</v>
       </c>
       <c r="O24" s="12">
-        <f>IF($N24=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P24" s="12">
-        <f>IF($N24=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q24" s="12">
-        <f>IF($N24=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R24" s="12">
-        <f>IF($N24=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T24">
@@ -2519,19 +2520,19 @@
         <v>4</v>
       </c>
       <c r="O25" s="12">
-        <f>IF($N25=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P25" s="12">
-        <f>IF($N25=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q25" s="12">
-        <f>IF($N25=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R25" s="12">
-        <f>IF($N25=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2565,19 +2566,19 @@
         <v>2</v>
       </c>
       <c r="O26" s="12">
-        <f>IF($N26=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P26" s="12">
-        <f>IF($N26=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q26" s="12">
-        <f>IF($N26=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R26" s="12">
-        <f>IF($N26=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2614,19 +2615,19 @@
         <v>2</v>
       </c>
       <c r="O27" s="12">
-        <f>IF($N27=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P27" s="12">
-        <f>IF($N27=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q27" s="12">
-        <f>IF($N27=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R27" s="12">
-        <f>IF($N27=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2660,19 +2661,19 @@
       </c>
       <c r="M28" s="5"/>
       <c r="O28" s="12">
-        <f>IF($N28=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P28" s="12">
-        <f>IF($N28=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q28" s="12">
-        <f>IF($N28=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="12">
-        <f>IF($N28=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2701,19 +2702,19 @@
       </c>
       <c r="M29" s="5"/>
       <c r="O29" s="12">
-        <f>IF($N29=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P29" s="12">
-        <f>IF($N29=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q29" s="12">
-        <f>IF($N29=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="12">
-        <f>IF($N29=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2748,19 +2749,19 @@
         <v>1</v>
       </c>
       <c r="O30" s="12">
-        <f>IF($N30=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P30" s="12">
-        <f>IF($N30=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q30" s="12">
-        <f>IF($N30=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="12">
-        <f>IF($N30=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2792,19 +2793,19 @@
         <v>3</v>
       </c>
       <c r="O31" s="12">
-        <f>IF($N31=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P31" s="12">
-        <f>IF($N31=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q31" s="12">
-        <f>IF($N31=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R31" s="12">
-        <f>IF($N31=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2844,19 +2845,19 @@
         <v>3</v>
       </c>
       <c r="O32" s="12">
-        <f>IF($N32=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P32" s="12">
-        <f>IF($N32=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q32" s="12">
-        <f>IF($N32=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R32" s="12">
-        <f>IF($N32=R$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_15 декабря 2023 г. 8:49:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -263,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,6 +302,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -412,11 +415,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="162406360"/>
-        <c:axId val="162407776"/>
+        <c:axId val="114291784"/>
+        <c:axId val="153500376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162406360"/>
+        <c:axId val="114291784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +461,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162407776"/>
+        <c:crossAx val="153500376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -466,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162407776"/>
+        <c:axId val="153500376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +520,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162406360"/>
+        <c:crossAx val="114291784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1435,7 +1438,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2291,6 +2294,12 @@
       <c r="I19" s="6">
         <v>5</v>
       </c>
+      <c r="J19" s="18">
+        <v>5</v>
+      </c>
+      <c r="K19" s="18">
+        <v>5</v>
+      </c>
       <c r="M19" s="5"/>
       <c r="N19">
         <v>1</v>
@@ -2310,6 +2319,9 @@
       <c r="R19" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_15 декабря 2023 г. 9:05:36_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -415,11 +415,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="114291784"/>
-        <c:axId val="153500376"/>
+        <c:axId val="163086072"/>
+        <c:axId val="163088032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114291784"/>
+        <c:axId val="163086072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153500376"/>
+        <c:crossAx val="163088032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153500376"/>
+        <c:axId val="163088032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +520,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114291784"/>
+        <c:crossAx val="163086072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1438,7 +1438,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_15 декабря 2023 г. 9:11:06_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -415,11 +415,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="163086072"/>
-        <c:axId val="163088032"/>
+        <c:axId val="154262936"/>
+        <c:axId val="154263320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="163086072"/>
+        <c:axId val="154262936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163088032"/>
+        <c:crossAx val="154263320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163088032"/>
+        <c:axId val="154263320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +520,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163086072"/>
+        <c:crossAx val="154262936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1438,7 +1438,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1578,6 +1578,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">

</xml_diff>

<commit_message>
AutoCommit_15 декабря 2023 г. 12:09:17_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>ДифЗачёт</t>
+  </si>
+  <si>
+    <t>ы</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -303,6 +306,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -415,11 +424,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="154262936"/>
-        <c:axId val="154263320"/>
+        <c:axId val="126465248"/>
+        <c:axId val="126466816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154262936"/>
+        <c:axId val="126465248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +470,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154263320"/>
+        <c:crossAx val="126466816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +478,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154263320"/>
+        <c:axId val="126466816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +529,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154262936"/>
+        <c:crossAx val="126465248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1438,7 +1447,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1699,6 +1708,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1732,6 +1744,9 @@
       <c r="J7" s="6">
         <v>5</v>
       </c>
+      <c r="K7" s="18">
+        <v>5</v>
+      </c>
       <c r="M7" s="5"/>
       <c r="N7">
         <v>4</v>
@@ -1752,6 +1767,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1783,6 +1801,12 @@
         <v>5</v>
       </c>
       <c r="J8" s="6">
+        <v>5</v>
+      </c>
+      <c r="K8" s="18">
+        <v>5</v>
+      </c>
+      <c r="L8" s="18">
         <v>5</v>
       </c>
       <c r="M8" s="5"/>
@@ -1919,6 +1943,16 @@
       <c r="H11" s="6">
         <v>5</v>
       </c>
+      <c r="I11" s="18">
+        <v>5</v>
+      </c>
+      <c r="J11" s="18">
+        <v>5</v>
+      </c>
+      <c r="K11" s="18">
+        <v>5</v>
+      </c>
+      <c r="L11" s="13"/>
       <c r="M11" s="5"/>
       <c r="N11">
         <v>1</v>
@@ -1938,6 +1972,9 @@
       <c r="R11" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2056,7 +2093,9 @@
       <c r="J14" s="7">
         <v>5</v>
       </c>
-      <c r="K14" s="13"/>
+      <c r="K14" s="13">
+        <v>5</v>
+      </c>
       <c r="M14" s="5"/>
       <c r="N14">
         <v>2</v>
@@ -2194,6 +2233,12 @@
       <c r="J17" s="6">
         <v>5</v>
       </c>
+      <c r="K17" s="20">
+        <v>5</v>
+      </c>
+      <c r="L17" s="19">
+        <v>5</v>
+      </c>
       <c r="M17" s="5"/>
       <c r="N17">
         <v>1</v>
@@ -2213,6 +2258,9 @@
       <c r="R17" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2356,6 +2404,13 @@
       <c r="I20" s="6">
         <v>5</v>
       </c>
+      <c r="J20" s="20">
+        <v>5</v>
+      </c>
+      <c r="K20" s="20">
+        <v>5</v>
+      </c>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
       <c r="O20" s="12">
         <f t="shared" si="1"/>
@@ -2372,6 +2427,9 @@
       <c r="R20" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2453,6 +2511,9 @@
       <c r="I22" s="6">
         <v>5</v>
       </c>
+      <c r="K22" s="19">
+        <v>5</v>
+      </c>
       <c r="M22" s="5"/>
       <c r="N22">
         <v>1</v>
@@ -2472,6 +2533,9 @@
       <c r="R22" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T22">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2562,6 +2626,9 @@
       <c r="K24" s="7">
         <v>5</v>
       </c>
+      <c r="L24" s="20">
+        <v>5</v>
+      </c>
       <c r="M24" s="5"/>
       <c r="N24">
         <v>1</v>
@@ -2668,6 +2735,13 @@
       <c r="I26" s="6">
         <v>5</v>
       </c>
+      <c r="J26" s="19">
+        <v>5</v>
+      </c>
+      <c r="K26" s="19">
+        <v>5</v>
+      </c>
+      <c r="L26" s="13"/>
       <c r="M26" s="5"/>
       <c r="N26">
         <v>2</v>
@@ -2867,6 +2941,12 @@
       <c r="J30" s="6">
         <v>5</v>
       </c>
+      <c r="K30" s="20">
+        <v>5</v>
+      </c>
+      <c r="L30" s="20">
+        <v>5</v>
+      </c>
       <c r="M30" s="5"/>
       <c r="N30">
         <v>1</v>
@@ -2886,6 +2966,9 @@
       <c r="R30" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T30">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2989,6 +3072,9 @@
       <c r="R32" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="4:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 12:35:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -421,11 +421,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="105186568"/>
-        <c:axId val="105186952"/>
+        <c:axId val="154308968"/>
+        <c:axId val="154311408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105186568"/>
+        <c:axId val="154308968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +467,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105186952"/>
+        <c:crossAx val="154311408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105186952"/>
+        <c:axId val="154311408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +526,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105186568"/>
+        <c:crossAx val="154308968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1441,10 +1441,10 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2003,6 +2003,13 @@
       <c r="I12" s="6">
         <v>5</v>
       </c>
+      <c r="J12" s="18">
+        <v>5</v>
+      </c>
+      <c r="K12" s="13">
+        <v>5</v>
+      </c>
+      <c r="L12" s="13"/>
       <c r="M12" s="5"/>
       <c r="N12">
         <v>3</v>
@@ -2176,7 +2183,18 @@
       <c r="F16" s="6">
         <v>5</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="19">
+        <v>5</v>
+      </c>
+      <c r="I16" s="18">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
       <c r="M16" s="5"/>
       <c r="N16">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 14:21:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>ДифЗачёт</t>
+  </si>
+  <si>
+    <t>ДОМАШКА</t>
+  </si>
+  <si>
+    <t>БЕЗ ДОМАШКИ МИНУС БАЛ</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,6 +321,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -421,11 +439,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="154308968"/>
-        <c:axId val="154311408"/>
+        <c:axId val="154992984"/>
+        <c:axId val="154989456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154308968"/>
+        <c:axId val="154992984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +485,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154311408"/>
+        <c:crossAx val="154989456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154311408"/>
+        <c:axId val="154989456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +544,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154308968"/>
+        <c:crossAx val="154992984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1438,13 +1456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1456,12 +1474,12 @@
     <col min="15" max="18" width="3.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1526,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1530,7 +1548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>IF(B4=C4,1,"______")</f>
         <v>1</v>
@@ -1588,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>IF(B5=C5,A4+1,"______")</f>
         <v>2</v>
@@ -1650,7 +1668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A31" si="2">IF(B6=C6,A5+1,"______")</f>
         <v>3</v>
@@ -1709,7 +1727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1768,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1826,8 +1844,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1879,8 +1900,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1914,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1974,7 +1998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -2030,8 +2054,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -2065,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -2121,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2162,8 +2189,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <v>5</v>
+      </c>
+      <c r="U15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -2195,6 +2228,9 @@
       <c r="J16">
         <v>5</v>
       </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
       <c r="M16" s="5"/>
       <c r="N16">
         <v>3</v>
@@ -2215,8 +2251,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -2278,7 +2317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -2331,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -2390,7 +2429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -2447,7 +2486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -2497,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -2526,7 +2565,13 @@
       <c r="I22" s="6">
         <v>5</v>
       </c>
-      <c r="K22" s="19">
+      <c r="J22" s="21">
+        <v>5</v>
+      </c>
+      <c r="K22" s="22">
+        <v>5</v>
+      </c>
+      <c r="L22" s="22">
         <v>5</v>
       </c>
       <c r="M22" s="5"/>
@@ -2553,7 +2598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -2605,8 +2650,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <v>5</v>
+      </c>
+      <c r="U23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -2668,7 +2719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -2721,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -2777,8 +2828,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -2831,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -2880,8 +2934,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -2895,7 +2952,9 @@
       <c r="D29" s="6">
         <v>5</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
       <c r="F29" s="6">
         <v>5</v>
       </c>
@@ -2908,6 +2967,13 @@
       <c r="I29" s="6">
         <v>5</v>
       </c>
+      <c r="J29" s="20">
+        <v>5</v>
+      </c>
+      <c r="K29" s="20">
+        <v>5</v>
+      </c>
+      <c r="L29" s="20"/>
       <c r="M29" s="5"/>
       <c r="O29" s="12">
         <f t="shared" si="1"/>
@@ -2926,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -2986,7 +3052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3034,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 15:04:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -439,11 +439,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="154992984"/>
-        <c:axId val="154989456"/>
+        <c:axId val="153400272"/>
+        <c:axId val="154380360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154992984"/>
+        <c:axId val="153400272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +485,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154989456"/>
+        <c:crossAx val="154380360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154989456"/>
+        <c:axId val="154380360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +544,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154992984"/>
+        <c:crossAx val="153400272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,10 +1459,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="R3" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2884,6 +2884,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="T27">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -2975,6 +2978,9 @@
       </c>
       <c r="L29" s="20"/>
       <c r="M29" s="5"/>
+      <c r="N29" s="19">
+        <v>4</v>
+      </c>
       <c r="O29" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2989,7 +2995,10 @@
       </c>
       <c r="R29" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 12:45:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -272,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,6 +324,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -436,11 +439,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="113338456"/>
-        <c:axId val="114511376"/>
+        <c:axId val="147767312"/>
+        <c:axId val="148156688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113338456"/>
+        <c:axId val="147767312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +485,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114511376"/>
+        <c:crossAx val="148156688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114511376"/>
+        <c:axId val="148156688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +544,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113338456"/>
+        <c:crossAx val="147767312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,7 +1462,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
+      <selection pane="bottomRight" activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3087,7 +3090,16 @@
       <c r="H31" s="6">
         <v>5</v>
       </c>
-      <c r="I31" s="2"/>
+      <c r="I31" s="23">
+        <v>5</v>
+      </c>
+      <c r="J31" s="20">
+        <v>5</v>
+      </c>
+      <c r="K31" s="19">
+        <v>5</v>
+      </c>
+      <c r="L31" s="19"/>
       <c r="M31" s="5"/>
       <c r="N31">
         <v>3</v>
@@ -3107,6 +3119,9 @@
       <c r="R31" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="T31">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 15:48:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -439,11 +439,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="147767312"/>
-        <c:axId val="148156688"/>
+        <c:axId val="161825720"/>
+        <c:axId val="126546472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147767312"/>
+        <c:axId val="161825720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +485,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148156688"/>
+        <c:crossAx val="126546472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148156688"/>
+        <c:axId val="126546472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +544,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147767312"/>
+        <c:crossAx val="161825720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,10 +1459,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U31" sqref="U31"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1880,10 @@
       <c r="J9" s="6">
         <v>5</v>
       </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19">
+        <v>5</v>
+      </c>
       <c r="M9" s="5"/>
       <c r="N9">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 13:11:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -439,11 +439,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="103854544"/>
-        <c:axId val="147801696"/>
+        <c:axId val="126761144"/>
+        <c:axId val="147915192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103854544"/>
+        <c:axId val="126761144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +485,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147801696"/>
+        <c:crossAx val="147915192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147801696"/>
+        <c:axId val="147915192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +544,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103854544"/>
+        <c:crossAx val="126761144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1462,7 +1462,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U25" sqref="U25"/>
+      <selection pane="bottomRight" activeCell="L23" sqref="K23:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2646,6 +2646,12 @@
       <c r="J23" s="6">
         <v>5</v>
       </c>
+      <c r="K23" s="20">
+        <v>5</v>
+      </c>
+      <c r="L23" s="20">
+        <v>5</v>
+      </c>
       <c r="M23" s="5"/>
       <c r="N23">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 16:41:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,11 +165,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -275,16 +270,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -312,8 +304,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -442,11 +434,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="130797336"/>
-        <c:axId val="161068088"/>
+        <c:axId val="165405712"/>
+        <c:axId val="166183880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130797336"/>
+        <c:axId val="165405712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +480,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161068088"/>
+        <c:crossAx val="166183880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161068088"/>
+        <c:axId val="166183880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +539,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130797336"/>
+        <c:crossAx val="165405712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,13 +1451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomRight" activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1470,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1495,22 +1487,22 @@
       <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="O2">
@@ -1525,7 +1517,7 @@
       <c r="R2">
         <v>4</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1538,15 +1530,15 @@
         <f>SUM(O4:O33)</f>
         <v>6</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <f t="shared" ref="P3:R3" si="0">SUM(P4:P33)</f>
         <v>5</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R3" s="12">
+        <v>8</v>
+      </c>
+      <c r="R3" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1562,46 +1554,46 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6">
-        <v>5</v>
-      </c>
-      <c r="F4" s="6">
-        <v>5</v>
-      </c>
-      <c r="G4" s="6">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6">
-        <v>5</v>
-      </c>
-      <c r="I4" s="6">
-        <v>5</v>
-      </c>
-      <c r="J4" s="6">
-        <v>5</v>
-      </c>
-      <c r="K4" s="7">
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>5</v>
+      </c>
+      <c r="J4" s="5">
+        <v>5</v>
+      </c>
+      <c r="K4" s="6">
         <v>5</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:R32" si="1">IF($N4=O$2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q4" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R4" s="12">
+        <f t="shared" ref="O4:R41" si="1">IF($N4=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1620,50 +1612,50 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6">
-        <v>5</v>
-      </c>
-      <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>5</v>
-      </c>
-      <c r="I5" s="6">
-        <v>5</v>
-      </c>
-      <c r="J5" s="7">
-        <v>5</v>
-      </c>
-      <c r="K5" s="6">
-        <v>5</v>
-      </c>
-      <c r="L5" s="7">
-        <v>5</v>
-      </c>
-      <c r="M5" s="5"/>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>5</v>
+      </c>
+      <c r="L5" s="6">
+        <v>5</v>
+      </c>
+      <c r="M5" s="4"/>
       <c r="N5">
         <v>4</v>
       </c>
-      <c r="O5" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="12">
+      <c r="O5" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1682,47 +1674,47 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="6">
-        <v>5</v>
-      </c>
-      <c r="J6" s="7">
-        <v>5</v>
-      </c>
-      <c r="K6" s="7">
-        <v>5</v>
-      </c>
-      <c r="M6" s="5"/>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="6">
+        <v>5</v>
+      </c>
+      <c r="M6" s="4"/>
       <c r="N6">
         <v>4</v>
       </c>
-      <c r="O6" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="12">
+      <c r="O6" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1741,47 +1733,47 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="6">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6">
-        <v>5</v>
-      </c>
-      <c r="H7" s="6">
-        <v>5</v>
-      </c>
-      <c r="I7" s="6">
-        <v>5</v>
-      </c>
-      <c r="J7" s="6">
-        <v>5</v>
-      </c>
-      <c r="K7" s="18">
-        <v>5</v>
-      </c>
-      <c r="M7" s="5"/>
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5">
+        <v>5</v>
+      </c>
+      <c r="K7" s="17">
+        <v>5</v>
+      </c>
+      <c r="M7" s="4"/>
       <c r="N7">
         <v>4</v>
       </c>
-      <c r="O7" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="12">
+      <c r="O7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1800,50 +1792,50 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>5</v>
-      </c>
-      <c r="I8" s="6">
-        <v>5</v>
-      </c>
-      <c r="J8" s="6">
-        <v>5</v>
-      </c>
-      <c r="K8" s="18">
-        <v>5</v>
-      </c>
-      <c r="L8" s="18">
-        <v>5</v>
-      </c>
-      <c r="M8" s="5"/>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5">
+        <v>5</v>
+      </c>
+      <c r="K8" s="17">
+        <v>5</v>
+      </c>
+      <c r="L8" s="17">
+        <v>5</v>
+      </c>
+      <c r="M8" s="4"/>
       <c r="N8">
         <v>3</v>
       </c>
-      <c r="O8" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R8" s="12">
+      <c r="O8" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1862,48 +1854,48 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6">
-        <v>5</v>
-      </c>
-      <c r="F9" s="6">
-        <v>5</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="6">
-        <v>5</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5</v>
-      </c>
-      <c r="J9" s="6">
-        <v>5</v>
-      </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19">
-        <v>5</v>
-      </c>
-      <c r="M9" s="5"/>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5</v>
+      </c>
+      <c r="I9" s="5">
+        <v>5</v>
+      </c>
+      <c r="J9" s="5">
+        <v>5</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18">
+        <v>5</v>
+      </c>
+      <c r="M9" s="4"/>
       <c r="N9">
         <v>3</v>
       </c>
-      <c r="O9" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R9" s="12">
+      <c r="O9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R9" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1911,36 +1903,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="9" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9">
-        <v>5</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="O10" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="12">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8">
+        <v>5</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="O10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1956,48 +1948,48 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6">
-        <v>5</v>
-      </c>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6">
-        <v>5</v>
-      </c>
-      <c r="H11" s="6">
-        <v>5</v>
-      </c>
-      <c r="I11" s="18">
-        <v>5</v>
-      </c>
-      <c r="J11" s="18">
-        <v>5</v>
-      </c>
-      <c r="K11" s="18">
-        <v>5</v>
-      </c>
-      <c r="L11" s="13"/>
-      <c r="M11" s="5"/>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5</v>
+      </c>
+      <c r="I11" s="17">
+        <v>5</v>
+      </c>
+      <c r="J11" s="17">
+        <v>5</v>
+      </c>
+      <c r="K11" s="17">
+        <v>5</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="4"/>
       <c r="N11">
         <v>1</v>
       </c>
-      <c r="O11" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P11" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="12">
+      <c r="O11" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2016,48 +2008,48 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="6">
-        <v>5</v>
-      </c>
-      <c r="E12" s="6">
-        <v>5</v>
-      </c>
-      <c r="F12" s="6">
-        <v>5</v>
-      </c>
-      <c r="G12" s="6">
-        <v>5</v>
-      </c>
-      <c r="H12" s="6">
-        <v>5</v>
-      </c>
-      <c r="I12" s="6">
-        <v>5</v>
-      </c>
-      <c r="J12" s="18">
-        <v>5</v>
-      </c>
-      <c r="K12" s="13">
-        <v>5</v>
-      </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="5"/>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
+        <v>5</v>
+      </c>
+      <c r="I12" s="5">
+        <v>5</v>
+      </c>
+      <c r="J12" s="17">
+        <v>5</v>
+      </c>
+      <c r="K12" s="12">
+        <v>5</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="4"/>
       <c r="N12">
         <v>3</v>
       </c>
-      <c r="O12" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="12">
+      <c r="O12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2065,36 +2057,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="9" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
-        <v>5</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="O13" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="12">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="O13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2110,47 +2102,47 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6">
-        <v>5</v>
-      </c>
-      <c r="E14" s="6">
-        <v>5</v>
-      </c>
-      <c r="F14" s="6">
-        <v>5</v>
-      </c>
-      <c r="G14" s="6">
-        <v>5</v>
-      </c>
-      <c r="H14" s="7">
-        <v>5</v>
-      </c>
-      <c r="I14" s="7">
-        <v>5</v>
-      </c>
-      <c r="J14" s="7">
-        <v>5</v>
-      </c>
-      <c r="K14" s="13">
-        <v>5</v>
-      </c>
-      <c r="M14" s="5"/>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="6">
+        <v>5</v>
+      </c>
+      <c r="I14" s="6">
+        <v>5</v>
+      </c>
+      <c r="J14" s="6">
+        <v>5</v>
+      </c>
+      <c r="K14" s="12">
+        <v>5</v>
+      </c>
+      <c r="M14" s="4"/>
       <c r="N14">
         <v>2</v>
       </c>
-      <c r="O14" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="12">
+      <c r="O14" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2172,39 +2164,39 @@
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="6">
-        <v>5</v>
-      </c>
-      <c r="E15" s="6">
-        <v>5</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="I15" s="6">
-        <v>5</v>
-      </c>
-      <c r="J15" s="20">
-        <v>5</v>
-      </c>
-      <c r="K15" s="20">
-        <v>5</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="O15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="12">
+      <c r="I15" s="5">
+        <v>5</v>
+      </c>
+      <c r="J15" s="19">
+        <v>5</v>
+      </c>
+      <c r="K15" s="19">
+        <v>5</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="O15" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2223,22 +2215,22 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="6">
-        <v>5</v>
-      </c>
-      <c r="E16" s="6">
-        <v>5</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5">
         <v>5</v>
       </c>
       <c r="G16" s="2">
         <v>5</v>
       </c>
-      <c r="H16" s="19">
-        <v>5</v>
-      </c>
-      <c r="I16" s="18">
+      <c r="H16" s="18">
+        <v>5</v>
+      </c>
+      <c r="I16" s="17">
         <v>5</v>
       </c>
       <c r="J16">
@@ -2247,23 +2239,23 @@
       <c r="K16">
         <v>5</v>
       </c>
-      <c r="M16" s="5"/>
+      <c r="M16" s="4"/>
       <c r="N16">
         <v>3</v>
       </c>
-      <c r="O16" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="12">
+      <c r="O16" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2282,50 +2274,50 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="6">
-        <v>5</v>
-      </c>
-      <c r="E17" s="6">
-        <v>5</v>
-      </c>
-      <c r="F17" s="6">
-        <v>5</v>
-      </c>
-      <c r="G17" s="6">
-        <v>5</v>
-      </c>
-      <c r="H17" s="6">
-        <v>5</v>
-      </c>
-      <c r="I17" s="6">
-        <v>5</v>
-      </c>
-      <c r="J17" s="6">
-        <v>5</v>
-      </c>
-      <c r="K17" s="20">
-        <v>5</v>
-      </c>
-      <c r="L17" s="19">
-        <v>5</v>
-      </c>
-      <c r="M17" s="5"/>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" s="5">
+        <v>5</v>
+      </c>
+      <c r="I17" s="5">
+        <v>5</v>
+      </c>
+      <c r="J17" s="5">
+        <v>5</v>
+      </c>
+      <c r="K17" s="19">
+        <v>5</v>
+      </c>
+      <c r="L17" s="18">
+        <v>5</v>
+      </c>
+      <c r="M17" s="4"/>
       <c r="N17">
         <v>1</v>
       </c>
-      <c r="O17" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P17" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="12">
+      <c r="O17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2344,50 +2336,50 @@
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="6">
-        <v>5</v>
-      </c>
-      <c r="E18" s="6">
-        <v>5</v>
-      </c>
-      <c r="F18" s="6">
-        <v>5</v>
-      </c>
-      <c r="G18" s="6">
-        <v>5</v>
-      </c>
-      <c r="H18" s="6">
-        <v>5</v>
-      </c>
-      <c r="I18" s="6">
-        <v>5</v>
-      </c>
-      <c r="J18" s="6">
-        <v>5</v>
-      </c>
-      <c r="K18" s="7">
-        <v>5</v>
-      </c>
-      <c r="L18" s="7">
-        <v>5</v>
-      </c>
-      <c r="M18" s="5"/>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
+      <c r="F18" s="5">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5">
+        <v>5</v>
+      </c>
+      <c r="I18" s="5">
+        <v>5</v>
+      </c>
+      <c r="J18" s="5">
+        <v>5</v>
+      </c>
+      <c r="K18" s="6">
+        <v>5</v>
+      </c>
+      <c r="L18" s="6">
+        <v>5</v>
+      </c>
+      <c r="M18" s="4"/>
       <c r="N18">
         <v>4</v>
       </c>
-      <c r="O18" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="12">
+      <c r="O18" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2406,47 +2398,47 @@
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="6">
-        <v>5</v>
-      </c>
-      <c r="E19" s="6">
-        <v>5</v>
-      </c>
-      <c r="F19" s="6">
-        <v>5</v>
-      </c>
-      <c r="G19" s="6">
-        <v>5</v>
-      </c>
-      <c r="H19" s="6">
-        <v>5</v>
-      </c>
-      <c r="I19" s="6">
-        <v>5</v>
-      </c>
-      <c r="J19" s="18">
-        <v>5</v>
-      </c>
-      <c r="K19" s="18">
-        <v>5</v>
-      </c>
-      <c r="M19" s="5"/>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>5</v>
+      </c>
+      <c r="I19" s="5">
+        <v>5</v>
+      </c>
+      <c r="J19" s="17">
+        <v>5</v>
+      </c>
+      <c r="K19" s="17">
+        <v>5</v>
+      </c>
+      <c r="M19" s="4"/>
       <c r="N19">
         <v>1</v>
       </c>
-      <c r="O19" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P19" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="12">
+      <c r="O19" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P19" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2465,45 +2457,45 @@
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="6">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6">
-        <v>5</v>
-      </c>
-      <c r="F20" s="6">
-        <v>5</v>
-      </c>
-      <c r="G20" s="6">
-        <v>5</v>
-      </c>
-      <c r="H20" s="6">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6">
-        <v>5</v>
-      </c>
-      <c r="J20" s="20">
-        <v>5</v>
-      </c>
-      <c r="K20" s="20">
-        <v>5</v>
-      </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="5"/>
-      <c r="O20" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="12">
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
+      <c r="H20" s="5">
+        <v>5</v>
+      </c>
+      <c r="I20" s="5">
+        <v>5</v>
+      </c>
+      <c r="J20" s="19">
+        <v>5</v>
+      </c>
+      <c r="K20" s="19">
+        <v>5</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="4"/>
+      <c r="O20" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2522,41 +2514,41 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="6">
-        <v>5</v>
-      </c>
-      <c r="E21" s="6">
-        <v>5</v>
-      </c>
-      <c r="F21" s="6">
-        <v>5</v>
-      </c>
-      <c r="G21" s="6">
-        <v>5</v>
-      </c>
-      <c r="H21" s="6">
-        <v>5</v>
-      </c>
-      <c r="I21" s="6">
-        <v>5</v>
-      </c>
-      <c r="M21" s="5"/>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="5">
+        <v>5</v>
+      </c>
+      <c r="I21" s="5">
+        <v>5</v>
+      </c>
+      <c r="M21" s="4"/>
       <c r="N21">
         <v>3</v>
       </c>
-      <c r="O21" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R21" s="12">
+      <c r="O21" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2578,50 +2570,50 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="6">
-        <v>5</v>
-      </c>
-      <c r="E22" s="6">
-        <v>5</v>
-      </c>
-      <c r="F22" s="6">
-        <v>5</v>
-      </c>
-      <c r="G22" s="6">
-        <v>5</v>
-      </c>
-      <c r="H22" s="6">
-        <v>5</v>
-      </c>
-      <c r="I22" s="6">
-        <v>5</v>
-      </c>
-      <c r="J22" s="21">
-        <v>5</v>
-      </c>
-      <c r="K22" s="22">
-        <v>5</v>
-      </c>
-      <c r="L22" s="22">
-        <v>5</v>
-      </c>
-      <c r="M22" s="5"/>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
+      <c r="F22" s="5">
+        <v>5</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>5</v>
+      </c>
+      <c r="I22" s="5">
+        <v>5</v>
+      </c>
+      <c r="J22" s="20">
+        <v>5</v>
+      </c>
+      <c r="K22" s="21">
+        <v>5</v>
+      </c>
+      <c r="L22" s="21">
+        <v>5</v>
+      </c>
+      <c r="M22" s="4"/>
       <c r="N22">
         <v>1</v>
       </c>
-      <c r="O22" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P22" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="12">
+      <c r="O22" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2640,50 +2632,50 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
-        <v>5</v>
-      </c>
-      <c r="E23" s="6">
-        <v>5</v>
-      </c>
-      <c r="F23" s="6">
-        <v>5</v>
-      </c>
-      <c r="G23" s="6">
-        <v>5</v>
-      </c>
-      <c r="H23" s="7">
-        <v>5</v>
-      </c>
-      <c r="I23" s="6">
-        <v>5</v>
-      </c>
-      <c r="J23" s="6">
-        <v>5</v>
-      </c>
-      <c r="K23" s="20">
-        <v>5</v>
-      </c>
-      <c r="L23" s="20">
-        <v>5</v>
-      </c>
-      <c r="M23" s="5"/>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5</v>
+      </c>
+      <c r="F23" s="5">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5">
+        <v>5</v>
+      </c>
+      <c r="H23" s="6">
+        <v>5</v>
+      </c>
+      <c r="I23" s="5">
+        <v>5</v>
+      </c>
+      <c r="J23" s="5">
+        <v>5</v>
+      </c>
+      <c r="K23" s="19">
+        <v>5</v>
+      </c>
+      <c r="L23" s="19">
+        <v>5</v>
+      </c>
+      <c r="M23" s="4"/>
       <c r="N23">
         <v>2</v>
       </c>
-      <c r="O23" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q23" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="12">
+      <c r="O23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2705,50 +2697,50 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="6">
-        <v>5</v>
-      </c>
-      <c r="E24" s="6">
-        <v>5</v>
-      </c>
-      <c r="F24" s="6">
-        <v>5</v>
-      </c>
-      <c r="G24" s="6">
-        <v>5</v>
-      </c>
-      <c r="H24" s="6">
-        <v>5</v>
-      </c>
-      <c r="I24" s="6">
-        <v>5</v>
-      </c>
-      <c r="J24" s="6">
-        <v>5</v>
-      </c>
-      <c r="K24" s="7">
-        <v>5</v>
-      </c>
-      <c r="L24" s="20">
-        <v>5</v>
-      </c>
-      <c r="M24" s="5"/>
+      <c r="D24" s="5">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5</v>
+      </c>
+      <c r="F24" s="5">
+        <v>5</v>
+      </c>
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>5</v>
+      </c>
+      <c r="I24" s="5">
+        <v>5</v>
+      </c>
+      <c r="J24" s="5">
+        <v>5</v>
+      </c>
+      <c r="K24" s="6">
+        <v>5</v>
+      </c>
+      <c r="L24" s="19">
+        <v>5</v>
+      </c>
+      <c r="M24" s="4"/>
       <c r="N24">
         <v>1</v>
       </c>
-      <c r="O24" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P24" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="12">
+      <c r="O24" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2767,50 +2759,50 @@
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="6">
-        <v>5</v>
-      </c>
-      <c r="E25" s="6">
-        <v>5</v>
-      </c>
-      <c r="F25" s="6">
-        <v>5</v>
-      </c>
-      <c r="G25" s="6">
-        <v>5</v>
-      </c>
-      <c r="H25" s="6">
-        <v>5</v>
-      </c>
-      <c r="I25" s="6">
-        <v>5</v>
-      </c>
-      <c r="J25" s="6">
-        <v>5</v>
-      </c>
-      <c r="K25" s="20">
-        <v>5</v>
-      </c>
-      <c r="L25" s="19">
-        <v>5</v>
-      </c>
-      <c r="M25" s="19"/>
+      <c r="D25" s="5">
+        <v>5</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="5">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>5</v>
+      </c>
+      <c r="I25" s="5">
+        <v>5</v>
+      </c>
+      <c r="J25" s="5">
+        <v>5</v>
+      </c>
+      <c r="K25" s="19">
+        <v>5</v>
+      </c>
+      <c r="L25" s="18">
+        <v>5</v>
+      </c>
+      <c r="M25" s="18"/>
       <c r="N25">
         <v>4</v>
       </c>
-      <c r="O25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="12">
+      <c r="O25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2829,48 +2821,48 @@
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="6">
-        <v>5</v>
-      </c>
-      <c r="E26" s="6">
-        <v>5</v>
-      </c>
-      <c r="F26" s="6">
-        <v>5</v>
-      </c>
-      <c r="G26" s="6">
-        <v>5</v>
-      </c>
-      <c r="H26" s="6">
-        <v>5</v>
-      </c>
-      <c r="I26" s="6">
-        <v>5</v>
-      </c>
-      <c r="J26" s="19">
-        <v>5</v>
-      </c>
-      <c r="K26" s="19">
-        <v>5</v>
-      </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="5"/>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5">
+        <v>5</v>
+      </c>
+      <c r="G26" s="5">
+        <v>5</v>
+      </c>
+      <c r="H26" s="5">
+        <v>5</v>
+      </c>
+      <c r="I26" s="5">
+        <v>5</v>
+      </c>
+      <c r="J26" s="18">
+        <v>5</v>
+      </c>
+      <c r="K26" s="18">
+        <v>5</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="4"/>
       <c r="N26">
         <v>2</v>
       </c>
-      <c r="O26" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q26" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="12">
+      <c r="O26" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2889,44 +2881,44 @@
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="6">
-        <v>5</v>
-      </c>
-      <c r="E27" s="6">
-        <v>5</v>
-      </c>
-      <c r="F27" s="6">
-        <v>5</v>
-      </c>
-      <c r="G27" s="6">
-        <v>5</v>
-      </c>
-      <c r="H27" s="6">
-        <v>5</v>
-      </c>
-      <c r="I27" s="6">
-        <v>5</v>
-      </c>
-      <c r="J27" s="6">
-        <v>5</v>
-      </c>
-      <c r="M27" s="5"/>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5</v>
+      </c>
+      <c r="F27" s="5">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5</v>
+      </c>
+      <c r="I27" s="5">
+        <v>5</v>
+      </c>
+      <c r="J27" s="5">
+        <v>5</v>
+      </c>
+      <c r="M27" s="4"/>
       <c r="N27">
         <v>2</v>
       </c>
-      <c r="O27" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q27" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="12">
+      <c r="O27" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q27" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2945,41 +2937,41 @@
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="6">
-        <v>5</v>
-      </c>
-      <c r="E28" s="6">
-        <v>5</v>
-      </c>
-      <c r="F28" s="6">
-        <v>5</v>
-      </c>
-      <c r="G28" s="6">
-        <v>5</v>
-      </c>
-      <c r="H28" s="6">
-        <v>5</v>
-      </c>
-      <c r="I28" s="6">
-        <v>5</v>
-      </c>
-      <c r="J28" s="6">
-        <v>5</v>
-      </c>
-      <c r="M28" s="5"/>
-      <c r="O28" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="12">
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5">
+        <v>5</v>
+      </c>
+      <c r="F28" s="5">
+        <v>5</v>
+      </c>
+      <c r="G28" s="5">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5">
+        <v>5</v>
+      </c>
+      <c r="I28" s="5">
+        <v>5</v>
+      </c>
+      <c r="J28" s="5">
+        <v>5</v>
+      </c>
+      <c r="M28" s="4"/>
+      <c r="O28" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2998,48 +2990,48 @@
       <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="6">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="6">
-        <v>5</v>
-      </c>
-      <c r="G29" s="6">
-        <v>5</v>
-      </c>
-      <c r="H29" s="6">
-        <v>5</v>
-      </c>
-      <c r="I29" s="6">
-        <v>5</v>
-      </c>
-      <c r="J29" s="20">
-        <v>5</v>
-      </c>
-      <c r="K29" s="20">
-        <v>5</v>
-      </c>
-      <c r="L29" s="20"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="19">
+      <c r="D29" s="5">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
+      <c r="F29" s="5">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>5</v>
+      </c>
+      <c r="H29" s="5">
+        <v>5</v>
+      </c>
+      <c r="I29" s="5">
+        <v>5</v>
+      </c>
+      <c r="J29" s="19">
+        <v>5</v>
+      </c>
+      <c r="K29" s="19">
+        <v>5</v>
+      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="18">
         <v>4</v>
       </c>
-      <c r="O29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="12">
+      <c r="O29" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3058,48 +3050,48 @@
       <c r="C30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>5</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="6">
-        <v>5</v>
-      </c>
-      <c r="G30" s="6">
-        <v>5</v>
-      </c>
-      <c r="H30" s="6">
-        <v>5</v>
-      </c>
-      <c r="I30" s="6">
-        <v>5</v>
-      </c>
-      <c r="J30" s="6">
-        <v>5</v>
-      </c>
-      <c r="K30" s="20">
-        <v>5</v>
-      </c>
-      <c r="L30" s="20">
-        <v>5</v>
-      </c>
-      <c r="M30" s="5"/>
+      <c r="F30" s="5">
+        <v>5</v>
+      </c>
+      <c r="G30" s="5">
+        <v>5</v>
+      </c>
+      <c r="H30" s="5">
+        <v>5</v>
+      </c>
+      <c r="I30" s="5">
+        <v>5</v>
+      </c>
+      <c r="J30" s="5">
+        <v>5</v>
+      </c>
+      <c r="K30" s="19">
+        <v>5</v>
+      </c>
+      <c r="L30" s="19">
+        <v>5</v>
+      </c>
+      <c r="M30" s="4"/>
       <c r="N30">
         <v>1</v>
       </c>
-      <c r="O30" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P30" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="12">
+      <c r="O30" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P30" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3118,48 +3110,48 @@
       <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="6">
-        <v>5</v>
-      </c>
-      <c r="E31" s="6">
-        <v>5</v>
-      </c>
-      <c r="F31" s="6">
-        <v>5</v>
-      </c>
-      <c r="G31" s="6">
-        <v>5</v>
-      </c>
-      <c r="H31" s="6">
-        <v>5</v>
-      </c>
-      <c r="I31" s="23">
-        <v>5</v>
-      </c>
-      <c r="J31" s="20">
-        <v>5</v>
-      </c>
-      <c r="K31" s="19">
-        <v>5</v>
-      </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="5"/>
+      <c r="D31" s="5">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5</v>
+      </c>
+      <c r="F31" s="5">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5">
+        <v>5</v>
+      </c>
+      <c r="H31" s="5">
+        <v>5</v>
+      </c>
+      <c r="I31" s="22">
+        <v>5</v>
+      </c>
+      <c r="J31" s="19">
+        <v>5</v>
+      </c>
+      <c r="K31" s="18">
+        <v>5</v>
+      </c>
+      <c r="L31" s="18"/>
+      <c r="M31" s="4"/>
       <c r="N31">
         <v>3</v>
       </c>
-      <c r="O31" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R31" s="12">
+      <c r="O31" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R31" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3177,47 +3169,47 @@
       <c r="C32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="6">
-        <v>5</v>
-      </c>
-      <c r="E32" s="6">
-        <v>5</v>
-      </c>
-      <c r="F32" s="6">
-        <v>5</v>
-      </c>
-      <c r="G32" s="6">
-        <v>5</v>
-      </c>
-      <c r="H32" s="7">
-        <v>5</v>
-      </c>
-      <c r="I32" s="7">
-        <v>5</v>
-      </c>
-      <c r="J32" s="14">
-        <v>5</v>
-      </c>
-      <c r="K32" s="15">
-        <v>5</v>
-      </c>
-      <c r="M32" s="5"/>
+      <c r="D32" s="5">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5">
+        <v>5</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5</v>
+      </c>
+      <c r="I32" s="6">
+        <v>5</v>
+      </c>
+      <c r="J32" s="13">
+        <v>5</v>
+      </c>
+      <c r="K32" s="14">
+        <v>5</v>
+      </c>
+      <c r="M32" s="4"/>
       <c r="N32">
         <v>3</v>
       </c>
-      <c r="O32" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R32" s="12">
+      <c r="O32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3225,20 +3217,1053 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="4:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="3">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="33" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="5">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5">
+        <v>5</v>
+      </c>
+      <c r="F33" s="5">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5">
+        <v>5</v>
+      </c>
+      <c r="H33" s="6">
+        <v>5</v>
+      </c>
+      <c r="I33" s="6">
+        <v>5</v>
+      </c>
+      <c r="J33" s="13">
+        <v>5</v>
+      </c>
+      <c r="K33" s="14">
+        <v>5</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11">
+        <v>3</v>
+      </c>
+      <c r="O33" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="5">
+        <v>5</v>
+      </c>
+      <c r="E34" s="5">
+        <v>5</v>
+      </c>
+      <c r="F34" s="5">
+        <v>5</v>
+      </c>
+      <c r="G34" s="5">
+        <v>5</v>
+      </c>
+      <c r="H34" s="6">
+        <v>5</v>
+      </c>
+      <c r="I34" s="6">
+        <v>5</v>
+      </c>
+      <c r="J34" s="13">
+        <v>5</v>
+      </c>
+      <c r="K34" s="14">
+        <v>5</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11">
+        <v>3</v>
+      </c>
+      <c r="O34" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R34" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="5">
+        <v>5</v>
+      </c>
+      <c r="E35" s="5">
+        <v>5</v>
+      </c>
+      <c r="F35" s="5">
+        <v>5</v>
+      </c>
+      <c r="G35" s="5">
+        <v>5</v>
+      </c>
+      <c r="H35" s="6">
+        <v>5</v>
+      </c>
+      <c r="I35" s="6">
+        <v>5</v>
+      </c>
+      <c r="J35" s="13">
+        <v>5</v>
+      </c>
+      <c r="K35" s="14">
+        <v>5</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11">
+        <v>3</v>
+      </c>
+      <c r="O35" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R35" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="5">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5">
+        <v>5</v>
+      </c>
+      <c r="F36" s="5">
+        <v>5</v>
+      </c>
+      <c r="G36" s="5">
+        <v>5</v>
+      </c>
+      <c r="H36" s="6">
+        <v>5</v>
+      </c>
+      <c r="I36" s="6">
+        <v>5</v>
+      </c>
+      <c r="J36" s="13">
+        <v>5</v>
+      </c>
+      <c r="K36" s="14">
+        <v>5</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11">
+        <v>3</v>
+      </c>
+      <c r="O36" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R36" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="5">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>5</v>
+      </c>
+      <c r="G37" s="5">
+        <v>5</v>
+      </c>
+      <c r="H37" s="6">
+        <v>5</v>
+      </c>
+      <c r="I37" s="6">
+        <v>5</v>
+      </c>
+      <c r="J37" s="13">
+        <v>5</v>
+      </c>
+      <c r="K37" s="14">
+        <v>5</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11">
+        <v>3</v>
+      </c>
+      <c r="O37" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R37" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="5">
+        <v>5</v>
+      </c>
+      <c r="E38" s="5">
+        <v>5</v>
+      </c>
+      <c r="F38" s="5">
+        <v>5</v>
+      </c>
+      <c r="G38" s="5">
+        <v>5</v>
+      </c>
+      <c r="H38" s="6">
+        <v>5</v>
+      </c>
+      <c r="I38" s="6">
+        <v>5</v>
+      </c>
+      <c r="J38" s="13">
+        <v>5</v>
+      </c>
+      <c r="K38" s="14">
+        <v>5</v>
+      </c>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11">
+        <v>3</v>
+      </c>
+      <c r="O38" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R38" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="5">
+        <v>5</v>
+      </c>
+      <c r="E39" s="5">
+        <v>5</v>
+      </c>
+      <c r="F39" s="5">
+        <v>5</v>
+      </c>
+      <c r="G39" s="5">
+        <v>5</v>
+      </c>
+      <c r="H39" s="6">
+        <v>5</v>
+      </c>
+      <c r="I39" s="6">
+        <v>5</v>
+      </c>
+      <c r="J39" s="13">
+        <v>5</v>
+      </c>
+      <c r="K39" s="14">
+        <v>5</v>
+      </c>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11">
+        <v>3</v>
+      </c>
+      <c r="O39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="5">
+        <v>5</v>
+      </c>
+      <c r="E40" s="5">
+        <v>5</v>
+      </c>
+      <c r="F40" s="5">
+        <v>5</v>
+      </c>
+      <c r="G40" s="5">
+        <v>5</v>
+      </c>
+      <c r="H40" s="6">
+        <v>5</v>
+      </c>
+      <c r="I40" s="6">
+        <v>5</v>
+      </c>
+      <c r="J40" s="13">
+        <v>5</v>
+      </c>
+      <c r="K40" s="14">
+        <v>5</v>
+      </c>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11">
+        <v>3</v>
+      </c>
+      <c r="O40" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R40" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="5">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5">
+        <v>5</v>
+      </c>
+      <c r="F41" s="5">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5">
+        <v>5</v>
+      </c>
+      <c r="H41" s="6">
+        <v>5</v>
+      </c>
+      <c r="I41" s="6">
+        <v>5</v>
+      </c>
+      <c r="J41" s="13">
+        <v>5</v>
+      </c>
+      <c r="K41" s="14">
+        <v>5</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11">
+        <v>3</v>
+      </c>
+      <c r="O41" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11">
+        <v>5</v>
+      </c>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+    </row>
+    <row r="42" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="5">
+        <v>5</v>
+      </c>
+      <c r="E42" s="5">
+        <v>5</v>
+      </c>
+      <c r="F42" s="5">
+        <v>5</v>
+      </c>
+      <c r="G42" s="5">
+        <v>5</v>
+      </c>
+      <c r="H42" s="6">
+        <v>5</v>
+      </c>
+      <c r="I42" s="6">
+        <v>5</v>
+      </c>
+      <c r="J42" s="13">
+        <v>5</v>
+      </c>
+      <c r="K42" s="14">
+        <v>5</v>
+      </c>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11">
+        <v>3</v>
+      </c>
+      <c r="O42" s="11">
+        <f t="shared" ref="O42:R50" si="3">IF($N42=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R42" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11">
+        <v>5</v>
+      </c>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+    </row>
+    <row r="43" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="5">
+        <v>5</v>
+      </c>
+      <c r="E43" s="5">
+        <v>5</v>
+      </c>
+      <c r="F43" s="5">
+        <v>5</v>
+      </c>
+      <c r="G43" s="5">
+        <v>5</v>
+      </c>
+      <c r="H43" s="6">
+        <v>5</v>
+      </c>
+      <c r="I43" s="6">
+        <v>5</v>
+      </c>
+      <c r="J43" s="13">
+        <v>5</v>
+      </c>
+      <c r="K43" s="14">
+        <v>5</v>
+      </c>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11">
+        <v>3</v>
+      </c>
+      <c r="O43" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R43" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11">
+        <v>5</v>
+      </c>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+    </row>
+    <row r="44" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="5">
+        <v>5</v>
+      </c>
+      <c r="E44" s="5">
+        <v>5</v>
+      </c>
+      <c r="F44" s="5">
+        <v>5</v>
+      </c>
+      <c r="G44" s="5">
+        <v>5</v>
+      </c>
+      <c r="H44" s="6">
+        <v>5</v>
+      </c>
+      <c r="I44" s="6">
+        <v>5</v>
+      </c>
+      <c r="J44" s="13">
+        <v>5</v>
+      </c>
+      <c r="K44" s="14">
+        <v>5</v>
+      </c>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11">
+        <v>3</v>
+      </c>
+      <c r="O44" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R44" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11">
+        <v>5</v>
+      </c>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+    </row>
+    <row r="45" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="5">
+        <v>5</v>
+      </c>
+      <c r="E45" s="5">
+        <v>5</v>
+      </c>
+      <c r="F45" s="5">
+        <v>5</v>
+      </c>
+      <c r="G45" s="5">
+        <v>5</v>
+      </c>
+      <c r="H45" s="6">
+        <v>5</v>
+      </c>
+      <c r="I45" s="6">
+        <v>5</v>
+      </c>
+      <c r="J45" s="13">
+        <v>5</v>
+      </c>
+      <c r="K45" s="14">
+        <v>5</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11">
+        <v>3</v>
+      </c>
+      <c r="O45" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11">
+        <v>5</v>
+      </c>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+    </row>
+    <row r="46" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="5">
+        <v>5</v>
+      </c>
+      <c r="E46" s="5">
+        <v>5</v>
+      </c>
+      <c r="F46" s="5">
+        <v>5</v>
+      </c>
+      <c r="G46" s="5">
+        <v>5</v>
+      </c>
+      <c r="H46" s="6">
+        <v>5</v>
+      </c>
+      <c r="I46" s="6">
+        <v>5</v>
+      </c>
+      <c r="J46" s="13">
+        <v>5</v>
+      </c>
+      <c r="K46" s="14">
+        <v>5</v>
+      </c>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11">
+        <v>3</v>
+      </c>
+      <c r="O46" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R46" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11">
+        <v>5</v>
+      </c>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+    </row>
+    <row r="47" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="5">
+        <v>5</v>
+      </c>
+      <c r="E47" s="5">
+        <v>5</v>
+      </c>
+      <c r="F47" s="5">
+        <v>5</v>
+      </c>
+      <c r="G47" s="5">
+        <v>5</v>
+      </c>
+      <c r="H47" s="6">
+        <v>5</v>
+      </c>
+      <c r="I47" s="6">
+        <v>5</v>
+      </c>
+      <c r="J47" s="13">
+        <v>5</v>
+      </c>
+      <c r="K47" s="14">
+        <v>5</v>
+      </c>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11">
+        <v>3</v>
+      </c>
+      <c r="O47" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R47" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11">
+        <v>5</v>
+      </c>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+    </row>
+    <row r="48" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="5">
+        <v>5</v>
+      </c>
+      <c r="E48" s="5">
+        <v>5</v>
+      </c>
+      <c r="F48" s="5">
+        <v>5</v>
+      </c>
+      <c r="G48" s="5">
+        <v>5</v>
+      </c>
+      <c r="H48" s="6">
+        <v>5</v>
+      </c>
+      <c r="I48" s="6">
+        <v>5</v>
+      </c>
+      <c r="J48" s="13">
+        <v>5</v>
+      </c>
+      <c r="K48" s="14">
+        <v>5</v>
+      </c>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11">
+        <v>3</v>
+      </c>
+      <c r="O48" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R48" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11">
+        <v>5</v>
+      </c>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+    </row>
+    <row r="49" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="5">
+        <v>5</v>
+      </c>
+      <c r="E49" s="5">
+        <v>5</v>
+      </c>
+      <c r="F49" s="5">
+        <v>5</v>
+      </c>
+      <c r="G49" s="5">
+        <v>5</v>
+      </c>
+      <c r="H49" s="6">
+        <v>5</v>
+      </c>
+      <c r="I49" s="6">
+        <v>5</v>
+      </c>
+      <c r="J49" s="13">
+        <v>5</v>
+      </c>
+      <c r="K49" s="14">
+        <v>5</v>
+      </c>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11">
+        <v>3</v>
+      </c>
+      <c r="O49" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R49" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11">
+        <v>5</v>
+      </c>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+    </row>
+    <row r="50" spans="2:22" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="5">
+        <v>5</v>
+      </c>
+      <c r="E50" s="5">
+        <v>5</v>
+      </c>
+      <c r="F50" s="5">
+        <v>5</v>
+      </c>
+      <c r="G50" s="5">
+        <v>5</v>
+      </c>
+      <c r="H50" s="6">
+        <v>5</v>
+      </c>
+      <c r="I50" s="6">
+        <v>5</v>
+      </c>
+      <c r="J50" s="13">
+        <v>5</v>
+      </c>
+      <c r="K50" s="14">
+        <v>5</v>
+      </c>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11">
+        <v>3</v>
+      </c>
+      <c r="O50" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R50" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11">
+        <v>5</v>
+      </c>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+    </row>
+    <row r="51" spans="2:22" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AutoCommit_22 декабря 2023 г. 14:09:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ДисМат_.xlsx
+++ b/2ИСИП-222_ДисМат_.xlsx
@@ -166,6 +166,8 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="20"/>
@@ -434,11 +436,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165405712"/>
-        <c:axId val="166183880"/>
+        <c:axId val="210481112"/>
+        <c:axId val="210481504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165405712"/>
+        <c:axId val="210481112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +482,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166183880"/>
+        <c:crossAx val="210481504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -488,7 +490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166183880"/>
+        <c:axId val="210481504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,7 +541,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165405712"/>
+        <c:crossAx val="210481112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1454,10 +1456,10 @@
   <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T44" sqref="T44"/>
+      <selection pane="bottomRight" activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>